<commit_message>
PB overwiew is verbeterd & rapportage is in gang & contributie verder afmaken
</commit_message>
<xml_diff>
--- a/documentatie/Product backlog overview & Sprint backlogs(1).xlsx
+++ b/documentatie/Product backlog overview & Sprint backlogs(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6336" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -39508,7 +39508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -39723,7 +39723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>